<commit_message>
Error handling while running test cases
</commit_message>
<xml_diff>
--- a/TestCase Repository Test.xlsx
+++ b/TestCase Repository Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Test Case</t>
   </si>
@@ -148,6 +148,9 @@
  "voucher_type":"G",
  "voucher_refID": #random_string
 }</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +613,9 @@
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -637,7 +643,9 @@
         <v>34</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>

</xml_diff>